<commit_message>
Draw rough packet diagram of overall service
</commit_message>
<xml_diff>
--- a/TermProject/PacketDiagram/PacketDiagram.xlsx
+++ b/TermProject/PacketDiagram/PacketDiagram.xlsx
@@ -4,17 +4,24 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="717" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Test" sheetId="1" r:id="rId1"/>
+    <sheet name="Test" sheetId="1" state="hidden" r:id="rId1"/>
+    <sheet name="Connect" sheetId="2" r:id="rId2"/>
+    <sheet name="Login" sheetId="3" r:id="rId3"/>
+    <sheet name="LobbyList" sheetId="6" r:id="rId4"/>
+    <sheet name="LobbySelect" sheetId="4" r:id="rId5"/>
+    <sheet name="LobbySendMessage" sheetId="5" r:id="rId6"/>
+    <sheet name="LobbyUserList" sheetId="7" r:id="rId7"/>
+    <sheet name="LobbyExit" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
   <si>
     <t>TestReq</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -41,6 +48,166 @@
   </si>
   <si>
     <t>n</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>connect()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>accept()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LoginReq</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LoginRes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Version alpha</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>일단 무조건 통과</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>처리해야할 일들</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서버</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>User has</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>clientIdx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UserManager</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">User </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 유저매니저에 유저 추가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id, pw</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>success / fail</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>클라</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>id와 pw를 입력</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Send LoginReqPkt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Recv LoginResPkt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LobbySelect Scene으로 이동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LobbySelectScene 이동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>-&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Send LobbyListReqPkt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자동으로 요청</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LobbyListReq</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LobbyListRes</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lobby list</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1. 로비 리스트 보내기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자료구조</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>자료구조</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LobbyManager</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lobby has</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>users</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>meta info</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lobby id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Lobby</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>떠났을 때 제거</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -84,8 +251,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -420,6 +588,1253 @@
         <a:xfrm flipH="1" flipV="1">
           <a:off x="2162175" y="3819525"/>
           <a:ext cx="2914650" cy="28575"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="irc_mi" descr="https://thumbs.dreamstime.com/z/server-client-communication-2597991.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="40882" t="29729" r="40481" b="36856"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4810125" y="476250"/>
+          <a:ext cx="885825" cy="1295400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="irc_mi" descr="https://thumbs.dreamstime.com/z/server-client-communication-2597991.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="3207" t="33088" r="72545" b="42892"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="704850" y="695325"/>
+          <a:ext cx="1152525" cy="933450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="직선 화살표 연결선 3"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="3"/>
+          <a:endCxn id="2" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1857375" y="1123950"/>
+          <a:ext cx="2952750" cy="38100"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="직선 화살표 연결선 5"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="1876425" y="2495550"/>
+          <a:ext cx="2619375" cy="9525"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="irc_mi" descr="https://thumbs.dreamstime.com/z/server-client-communication-2597991.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="40882" t="29729" r="40481" b="36856"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4848225" y="1895475"/>
+          <a:ext cx="885825" cy="1295400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="irc_mi" descr="https://thumbs.dreamstime.com/z/server-client-communication-2597991.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="3207" t="33088" r="72545" b="42892"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="666750" y="2057400"/>
+          <a:ext cx="1152525" cy="933450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="irc_mi" descr="https://thumbs.dreamstime.com/z/server-client-communication-2597991.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="40882" t="29729" r="40481" b="36856"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4791075" y="628650"/>
+          <a:ext cx="885825" cy="1295400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="irc_mi" descr="https://thumbs.dreamstime.com/z/server-client-communication-2597991.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="3207" t="33088" r="72545" b="42892"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="685800" y="847725"/>
+          <a:ext cx="1152525" cy="933450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>542926</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>105087</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="직선 화살표 연결선 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1914526" y="1352551"/>
+          <a:ext cx="2705099" cy="9836"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="irc_mi" descr="https://thumbs.dreamstime.com/z/server-client-communication-2597991.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="40882" t="29729" r="40481" b="36856"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4848225" y="2400300"/>
+          <a:ext cx="885825" cy="1295400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="irc_mi" descr="https://thumbs.dreamstime.com/z/server-client-communication-2597991.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="3207" t="33088" r="72545" b="42892"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="742950" y="2619375"/>
+          <a:ext cx="1152525" cy="933450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>47626</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>193238</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>193238</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="직선 화살표 연결선 8"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2105026" y="3126938"/>
+          <a:ext cx="2571749" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="irc_mi" descr="https://thumbs.dreamstime.com/z/server-client-communication-2597991.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="40882" t="29729" r="40481" b="36856"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4791075" y="628650"/>
+          <a:ext cx="885825" cy="1295400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="irc_mi" descr="https://thumbs.dreamstime.com/z/server-client-communication-2597991.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="3207" t="33088" r="72545" b="42892"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="685800" y="847725"/>
+          <a:ext cx="1152525" cy="933450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>542926</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>105087</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="직선 화살표 연결선 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1914526" y="1352551"/>
+          <a:ext cx="2705099" cy="9836"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="irc_mi" descr="https://thumbs.dreamstime.com/z/server-client-communication-2597991.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="40882" t="29729" r="40481" b="36856"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4848225" y="2400300"/>
+          <a:ext cx="885825" cy="1295400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="irc_mi" descr="https://thumbs.dreamstime.com/z/server-client-communication-2597991.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="3207" t="33088" r="72545" b="42892"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="742950" y="2619375"/>
+          <a:ext cx="1152525" cy="933450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>47626</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>193238</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>193238</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="직선 화살표 연결선 6"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2105026" y="3126938"/>
+          <a:ext cx="2571749" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="irc_mi" descr="https://thumbs.dreamstime.com/z/server-client-communication-2597991.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="40882" t="29729" r="40481" b="36856"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4791075" y="628650"/>
+          <a:ext cx="885825" cy="1295400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="irc_mi" descr="https://thumbs.dreamstime.com/z/server-client-communication-2597991.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="3207" t="33088" r="72545" b="42892"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="685800" y="847725"/>
+          <a:ext cx="1152525" cy="933450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>542926</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>105087</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="직선 화살표 연결선 5"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1914526" y="1352551"/>
+          <a:ext cx="2705099" cy="9836"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="irc_mi" descr="https://thumbs.dreamstime.com/z/server-client-communication-2597991.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="40882" t="29729" r="40481" b="36856"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4848225" y="2400300"/>
+          <a:ext cx="885825" cy="1295400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="irc_mi" descr="https://thumbs.dreamstime.com/z/server-client-communication-2597991.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="3207" t="33088" r="72545" b="42892"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="742950" y="2619375"/>
+          <a:ext cx="1152525" cy="933450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>47626</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>193238</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>193238</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="직선 화살표 연결선 8"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="2105026" y="3126938"/>
+          <a:ext cx="2571749" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -737,7 +2152,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F9:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -783,4 +2198,338 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E5:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="5" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E3:P17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O9" sqref="O9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="5:16" x14ac:dyDescent="0.3">
+      <c r="E3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="5:16" x14ac:dyDescent="0.3">
+      <c r="E5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="5:16" x14ac:dyDescent="0.3">
+      <c r="J6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="5:16" x14ac:dyDescent="0.3">
+      <c r="N7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="5:16" x14ac:dyDescent="0.3">
+      <c r="J8" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="5:16" x14ac:dyDescent="0.3">
+      <c r="J9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="5:16" x14ac:dyDescent="0.3">
+      <c r="E12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="5:16" x14ac:dyDescent="0.3">
+      <c r="E14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="5:16" x14ac:dyDescent="0.3">
+      <c r="J15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E3:P17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="9" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="5:16" x14ac:dyDescent="0.3">
+      <c r="E3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="5:16" x14ac:dyDescent="0.3">
+      <c r="E5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="5:16" x14ac:dyDescent="0.3">
+      <c r="J6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="5:16" x14ac:dyDescent="0.3">
+      <c r="M7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="O7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="P7" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="5:16" x14ac:dyDescent="0.3">
+      <c r="O8" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="5:16" x14ac:dyDescent="0.3">
+      <c r="E12" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="5:16" x14ac:dyDescent="0.3">
+      <c r="E14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="5:16" x14ac:dyDescent="0.3">
+      <c r="J15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E2:E13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add a packet diagram
</commit_message>
<xml_diff>
--- a/TermProject/PacketDiagram/PacketDiagram.xlsx
+++ b/TermProject/PacketDiagram/PacketDiagram.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="717" firstSheet="1" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="717" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" state="hidden" r:id="rId1"/>
@@ -13,13 +13,14 @@
     <sheet name="LobbyUserList" sheetId="7" r:id="rId4"/>
     <sheet name="LobbyChatReq" sheetId="5" r:id="rId5"/>
     <sheet name="LobbyExit" sheetId="8" r:id="rId6"/>
+    <sheet name="RemoveUser" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="74">
   <si>
     <t>TestReq</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -294,6 +295,26 @@
   </si>
   <si>
     <t>Recv LoginNtf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RemoveUserNtf</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Client</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>받으면 해당 이름을 찾아서 삭제한다</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>UI -&gt; linked-list로 바꾸기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2144,6 +2165,164 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="irc_mi" descr="https://thumbs.dreamstime.com/z/server-client-communication-2597991.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="40882" t="29729" r="40481" b="36856"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="4105275" y="209550"/>
+          <a:ext cx="885825" cy="1295400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>200025</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="irc_mi" descr="https://thumbs.dreamstime.com/z/server-client-communication-2597991.jpg"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect l="3207" t="33088" r="72545" b="42892"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="2038350" y="2085975"/>
+          <a:ext cx="1152525" cy="933450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>76512</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="직선 화살표 연결선 3"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="3238500" y="2591112"/>
+          <a:ext cx="2762250" cy="9213"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 테마">
   <a:themeElements>
@@ -2513,7 +2692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
@@ -2807,8 +2986,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q16"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="P27" sqref="A17:P27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -3520,4 +3699,104 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:H18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>